<commit_message>
integration opik + cleaning + excel download
</commit_message>
<xml_diff>
--- a/app/storage/excel/Lead Tracking.xlsx
+++ b/app/storage/excel/Lead Tracking.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Lead Tracking" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="lead tracking1" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,6 +473,93 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Piotr P</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Technical Leader Allegro</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>500+</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Piotr P</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Technical Leader Allegro</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>500+</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>designation</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>total connection</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Piotr P</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Technical Leader Allegro</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>500+</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>